<commit_message>
readme + requirement + trip_id
</commit_message>
<xml_diff>
--- a/static/idfm_style/table_connection.xlsx
+++ b/static/idfm_style/table_connection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Desktop\2A Ponts ParisTech\S3-Mopsi\Git_project\Projet-MOPSI-2020\static\idfm_style\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EC5D51-8043-408D-B63F-640B52542150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38780423-84A9-49B9-BF07-9712785B494F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_connection" sheetId="1" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <t>TRAMWAY####T3B</t>
   </si>
   <si>
-    <t>TRAMWAY####T4</t>
-  </si>
-  <si>
     <t>TRAMWAY####T5</t>
   </si>
   <si>
@@ -410,6 +407,9 @@
   </si>
   <si>
     <t>TRAMWAY####T12</t>
+  </si>
+  <si>
+    <t>TRAIN####T4</t>
   </si>
 </sst>
 </file>
@@ -1252,18 +1252,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.86328125" customWidth="1"/>
-    <col min="4" max="4" width="39.73046875" customWidth="1"/>
-    <col min="5" max="5" width="60.73046875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>117</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>118</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>120</v>
       </c>
@@ -1858,12 +1858,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
@@ -1875,9 +1875,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -1892,9 +1892,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -1909,9 +1909,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -1926,9 +1926,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -1943,9 +1943,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -1960,9 +1960,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -1977,9 +1977,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
@@ -1994,9 +1994,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
         <v>24</v>
@@ -2011,7 +2011,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
bug Pyhton 3.9 lors de pip install -r requirement.txt sous windows
</commit_message>
<xml_diff>
--- a/static/idfm_style/table_connection.xlsx
+++ b/static/idfm_style/table_connection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Desktop\2A Ponts ParisTech\S3-Mopsi\Git_project\Projet-MOPSI-2020\static\idfm_style\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38780423-84A9-49B9-BF07-9712785B494F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C295EE3A-C220-4AF5-A059-864FB4112BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
     <t>TRAMWAY####T12</t>
   </si>
   <si>
-    <t>TRAIN####T4</t>
+    <t>TRAMWAY####T4</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1863,7 @@
         <v>129</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>

</xml_diff>